<commit_message>
updates to supp tables and code
added back in a study that was removed that shouldn't have been, reran models to get effect sizes with this study included again. General organisation of code
</commit_message>
<xml_diff>
--- a/ms/final model output and tables/Supplementary_models_S7-S12.xlsx
+++ b/ms/final model output and tables/Supplementary_models_S7-S12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_meta/ms/final model output and tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DB911A-4304-A94D-8AF5-73F3C6AC2165}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAE4398-BFE6-1843-9748-A19A3CFC893B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="19820" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
+    <workbookView xWindow="1680" yWindow="460" windowWidth="38300" windowHeight="19760" activeTab="1" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="7" r:id="rId1"/>
@@ -237,15 +237,6 @@
     <t>-0.99, 0.46</t>
   </si>
   <si>
-    <t>p=0.93</t>
-  </si>
-  <si>
-    <t>-0.75, 0.40</t>
-  </si>
-  <si>
-    <t>-0.53, 0.48</t>
-  </si>
-  <si>
     <t>p=0.90</t>
   </si>
   <si>
@@ -868,6 +859,15 @@
   </si>
   <si>
     <t>Here we include the same random effects as the intercept only models: study_ID (between study variance), phylo (phylogenetic variance) and obs (observation-level random effect - within study variance )</t>
+  </si>
+  <si>
+    <t>p=0.94</t>
+  </si>
+  <si>
+    <t>-0.75, 0.39</t>
+  </si>
+  <si>
+    <t>-0.52, 0.48</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997D318C-6FE4-1349-B40F-3ACEE7BB8369}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1345,77 +1345,77 @@
   <sheetData>
     <row r="1" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -1427,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9948B2D6-0D24-AC4F-B3C7-22D23935FFEB}">
   <dimension ref="A1:AN60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1443,23 +1443,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -1536,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2400.7800000000002</v>
+        <v>2749.45</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1758,10 +1758,10 @@
         <v>0.01</v>
       </c>
       <c r="C11">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="D11" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" s="4"/>
       <c r="I11" t="s">
@@ -1887,7 +1887,7 @@
         <v>0.41</v>
       </c>
       <c r="D13">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="I13" t="s">
         <v>15</v>
@@ -2113,19 +2113,19 @@
         <v>55</v>
       </c>
       <c r="D16">
-        <v>-0.6</v>
+        <v>-0.59</v>
       </c>
       <c r="E16">
-        <v>0.55000000000000004</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F16" s="31">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="G16" s="31">
         <v>74</v>
       </c>
       <c r="H16" s="31">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I16" t="s">
         <v>40</v>
@@ -2229,7 +2229,7 @@
         <v>54</v>
       </c>
       <c r="B17" s="13">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>56</v>
@@ -2368,7 +2368,7 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <v>3698.36</v>
+        <v>3775.07</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -2418,7 +2418,7 @@
         <v>0.01</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>276</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -2427,7 +2427,7 @@
         <v>0.02</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>8</v>
@@ -2436,7 +2436,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -2589,10 +2589,10 @@
         <v>0.01</v>
       </c>
       <c r="C23">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="D23" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -2648,7 +2648,7 @@
         <v>36</v>
       </c>
       <c r="B24">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="C24">
         <v>0.66</v>
@@ -2717,7 +2717,7 @@
         <v>0.65</v>
       </c>
       <c r="D25">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="I25" t="s">
         <v>15</v>
@@ -2940,7 +2940,7 @@
         <v>-0.18</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>69</v>
+        <v>277</v>
       </c>
       <c r="D28" s="7">
         <v>-0.61</v>
@@ -2949,13 +2949,13 @@
         <v>0.54</v>
       </c>
       <c r="F28" s="31">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="G28" s="31">
         <v>74</v>
       </c>
       <c r="H28" s="31">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I28" t="s">
         <v>40</v>
@@ -2964,7 +2964,7 @@
         <v>-0.04</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L28" s="26">
         <v>-0.64</v>
@@ -2988,7 +2988,7 @@
         <v>0.04</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="T28">
         <v>0.26</v>
@@ -3012,7 +3012,7 @@
         <v>0.03</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AB28" s="7">
         <v>0.22</v>
@@ -3036,7 +3036,7 @@
         <v>-0.03</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AJ28" s="7">
         <v>-0.14000000000000001</v>
@@ -3062,13 +3062,13 @@
         <v>-0.02</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>70</v>
+        <v>278</v>
       </c>
       <c r="D29" s="15">
         <v>-0.08</v>
       </c>
       <c r="E29" s="15">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="F29" s="13">
         <v>111</v>
@@ -3086,7 +3086,7 @@
         <v>0.01</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L29" s="13">
         <v>0.12</v>
@@ -3110,7 +3110,7 @@
         <v>-0.06</v>
       </c>
       <c r="S29" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="T29" s="15">
         <v>-0.37</v>
@@ -3158,7 +3158,7 @@
         <v>0.03</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AJ29" s="15">
         <v>0.14000000000000001</v>
@@ -3303,23 +3303,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -3446,7 +3446,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -3464,7 +3464,7 @@
         <v>0.03</v>
       </c>
       <c r="S8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>8</v>
@@ -3473,7 +3473,7 @@
         <v>1</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -3482,7 +3482,7 @@
         <v>0.02</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -3969,7 +3969,7 @@
         <v>-0.13</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D16">
         <v>-1.1000000000000001</v>
@@ -3993,7 +3993,7 @@
         <v>-0.05</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L16" s="28">
         <v>-0.3</v>
@@ -4017,7 +4017,7 @@
         <v>0.24</v>
       </c>
       <c r="S16" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T16" s="4">
         <v>1.74</v>
@@ -4065,7 +4065,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AJ16" s="28">
         <v>0.87</v>
@@ -4091,7 +4091,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D17" s="13">
         <v>0</v>
@@ -4115,7 +4115,7 @@
         <v>0.26</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L17" s="13">
         <v>1.08</v>
@@ -4139,7 +4139,7 @@
         <v>-0.03</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="T17" s="15">
         <v>-0.18</v>
@@ -4163,7 +4163,7 @@
         <v>-0.09</v>
       </c>
       <c r="AA17" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AB17" s="13">
         <v>-1</v>
@@ -4187,7 +4187,7 @@
         <v>-0.05</v>
       </c>
       <c r="AI17" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AJ17" s="15">
         <v>-0.16</v>
@@ -4266,7 +4266,7 @@
         <v>77.59</v>
       </c>
       <c r="AI19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -4277,7 +4277,7 @@
         <v>0.08</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -4295,7 +4295,7 @@
         <v>0.06</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -4304,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="AA20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AG20" s="5" t="s">
         <v>8</v>
@@ -4313,7 +4313,7 @@
         <v>0.15</v>
       </c>
       <c r="AI20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -4799,7 +4799,7 @@
         <v>-0.15</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D28" s="7">
         <v>-0.56000000000000005</v>
@@ -4823,7 +4823,7 @@
         <v>-0.04</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L28" s="26">
         <v>-1.38</v>
@@ -4847,7 +4847,7 @@
         <v>-0.02</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="T28">
         <v>-0.39</v>
@@ -4871,7 +4871,7 @@
         <v>0.09</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AB28" s="7">
         <v>0.76</v>
@@ -4895,7 +4895,7 @@
         <v>0.06</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AJ28" s="7">
         <v>1.1399999999999999</v>
@@ -4921,7 +4921,7 @@
         <v>-0.03</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D29" s="13">
         <v>-0.28999999999999998</v>
@@ -4945,7 +4945,7 @@
         <v>-0.08</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L29" s="13">
         <v>-0.37</v>
@@ -4969,7 +4969,7 @@
         <v>-0.02</v>
       </c>
       <c r="S29" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="T29" s="15">
         <v>-0.24</v>
@@ -4993,7 +4993,7 @@
         <v>-0.09</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AB29" s="15">
         <v>-1.41</v>
@@ -5017,7 +5017,7 @@
         <v>-0.08</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AJ29" s="15">
         <v>-0.39</v>
@@ -5510,23 +5510,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -5653,7 +5653,7 @@
         <v>0.1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -5689,7 +5689,7 @@
         <v>0.1</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -6200,7 +6200,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L16">
         <v>-0.4</v>
@@ -6224,7 +6224,7 @@
         <v>0.15</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="T16">
         <v>0.76</v>
@@ -6248,7 +6248,7 @@
         <v>0.16</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AB16" s="5">
         <v>1</v>
@@ -6272,7 +6272,7 @@
         <v>0.08</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AJ16">
         <v>0.92</v>
@@ -6292,13 +6292,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B17" s="13">
         <v>0.08</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D17" s="13">
         <v>0.32</v>
@@ -6316,13 +6316,13 @@
         <v>16</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J17" s="13">
         <v>0.05</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L17" s="13">
         <v>0.6</v>
@@ -6340,13 +6340,13 @@
         <v>28</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R17" s="15">
         <v>0.18</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="T17" s="15">
         <v>0.64</v>
@@ -6364,13 +6364,13 @@
         <v>21</v>
       </c>
       <c r="Y17" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Z17" s="13">
         <v>-0.16</v>
       </c>
       <c r="AA17" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AB17" s="13">
         <v>-1.48</v>
@@ -6388,13 +6388,13 @@
         <v>38</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AH17" s="15">
         <v>-0.05</v>
       </c>
       <c r="AI17" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AJ17" s="15">
         <v>-0.32</v>
@@ -6473,7 +6473,7 @@
         <v>77.27</v>
       </c>
       <c r="AI19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -6493,7 +6493,7 @@
         <v>2.39</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>8</v>
@@ -6502,7 +6502,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -7006,7 +7006,7 @@
         <v>-0.11</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D28" s="7">
         <v>-0.9</v>
@@ -7030,7 +7030,7 @@
         <v>-0.09</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L28" s="18">
         <v>-2.11</v>
@@ -7054,7 +7054,7 @@
         <v>0.01</v>
       </c>
       <c r="S28" s="27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="T28" s="26">
         <v>0.1</v>
@@ -7078,7 +7078,7 @@
         <v>0.11</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AB28" s="7">
         <v>0.73</v>
@@ -7102,7 +7102,7 @@
         <v>0.06</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="AJ28" s="7">
         <v>1.18</v>
@@ -7122,13 +7122,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B29" s="13">
         <v>0.15</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D29" s="13">
         <v>0.74</v>
@@ -7146,13 +7146,13 @@
         <v>16</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J29" s="13">
         <v>0.08</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L29" s="13">
         <v>1.55</v>
@@ -7170,13 +7170,13 @@
         <v>28</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R29" s="13">
         <v>-0.04</v>
       </c>
       <c r="S29" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="T29" s="13">
         <v>-0.54</v>
@@ -7194,13 +7194,13 @@
         <v>21</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Z29" s="15">
         <v>-0.09</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AB29" s="15">
         <v>-1.1399999999999999</v>
@@ -7218,13 +7218,13 @@
         <v>38</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AH29" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AJ29" s="15">
         <v>-0.65</v>
@@ -7268,23 +7268,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -7420,7 +7420,7 @@
         <v>0.15</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>8</v>
@@ -7441,7 +7441,7 @@
         <v>28</v>
       </c>
       <c r="AB8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -7937,7 +7937,7 @@
         <v>-0.12</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D16">
         <v>-0.85</v>
@@ -7961,7 +7961,7 @@
         <v>-0.06</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L16">
         <v>-0.35</v>
@@ -7985,7 +7985,7 @@
         <v>0.31</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T16">
         <v>1.2</v>
@@ -8009,7 +8009,7 @@
         <v>0.24</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AB16" s="5">
         <v>1.44</v>
@@ -8033,7 +8033,7 @@
         <v>-0.28999999999999998</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AJ16">
         <v>-1.24</v>
@@ -8053,13 +8053,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B17" s="13">
         <v>-0.02</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D17" s="13">
         <v>-0.14000000000000001</v>
@@ -8077,13 +8077,13 @@
         <v>22</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J17" s="13">
         <v>0.06</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L17" s="13">
         <v>0.39</v>
@@ -8101,13 +8101,13 @@
         <v>39</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R17" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="T17" s="15">
         <v>-0.31</v>
@@ -8125,13 +8125,13 @@
         <v>44</v>
       </c>
       <c r="Y17" s="29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Z17" s="29">
         <v>-0.31</v>
       </c>
       <c r="AA17" s="30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AB17" s="29">
         <v>-2.34</v>
@@ -8149,13 +8149,13 @@
         <v>40</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH17" s="13">
         <v>0.42</v>
       </c>
       <c r="AI17" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AJ17" s="13">
         <v>1.7</v>
@@ -8234,7 +8234,7 @@
         <v>77.55</v>
       </c>
       <c r="AI19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -8263,7 +8263,7 @@
         <v>0.23</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -8272,7 +8272,7 @@
         <v>0.6</v>
       </c>
       <c r="AA20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AG20" s="5" t="s">
         <v>8</v>
@@ -8281,7 +8281,7 @@
         <v>0.23</v>
       </c>
       <c r="AI20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -8767,7 +8767,7 @@
         <v>-0.13</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D28" s="7">
         <v>-1.05</v>
@@ -8791,7 +8791,7 @@
         <v>-0.1</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L28" s="26">
         <v>-1.18</v>
@@ -8815,7 +8815,7 @@
         <v>-0.08</v>
       </c>
       <c r="S28" s="27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="T28" s="26">
         <v>-0.57999999999999996</v>
@@ -8839,7 +8839,7 @@
         <v>0.11</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AB28" s="7">
         <v>0.73</v>
@@ -8863,7 +8863,7 @@
         <v>-0.01</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AJ28" s="7">
         <v>-7.0000000000000007E-2</v>
@@ -8883,13 +8883,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B29" s="13">
         <v>0.16</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D29" s="13">
         <v>0.93</v>
@@ -8907,13 +8907,13 @@
         <v>22</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J29" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L29" s="13">
         <v>0.75</v>
@@ -8931,13 +8931,13 @@
         <v>39</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R29" s="13">
         <v>0.06</v>
       </c>
       <c r="S29" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="T29" s="13">
         <v>0.47</v>
@@ -8955,13 +8955,13 @@
         <v>44</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Z29" s="15">
         <v>-0.08</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AB29" s="15">
         <v>-0.78</v>
@@ -8979,13 +8979,13 @@
         <v>40</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AH29" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AJ29" s="15">
         <v>0.48</v>
@@ -9036,23 +9036,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -9185,7 +9185,7 @@
         <v>1.38</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>8</v>
@@ -9200,10 +9200,10 @@
         <v>8.57</v>
       </c>
       <c r="AA8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB8" t="s">
         <v>155</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>158</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -9699,7 +9699,7 @@
         <v>-0.04</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D16">
         <v>-0.25</v>
@@ -9723,7 +9723,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L16" s="28">
         <v>-0.41</v>
@@ -9771,7 +9771,7 @@
         <v>0</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AB16" s="5">
         <v>0.03</v>
@@ -9795,7 +9795,7 @@
         <v>0.13</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AJ16" s="28">
         <v>1.1399999999999999</v>
@@ -9815,13 +9815,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B17" s="13">
         <v>-0.26</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D17" s="13">
         <v>-1.07</v>
@@ -9839,13 +9839,13 @@
         <v>94</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J17" s="13">
         <v>0.19</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L17" s="13">
         <v>1.17</v>
@@ -9863,7 +9863,7 @@
         <v>3</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="R17" s="15" t="s">
         <v>29</v>
@@ -9887,13 +9887,13 @@
         <v>29</v>
       </c>
       <c r="Y17" s="29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Z17" s="29">
         <v>0.39</v>
       </c>
       <c r="AA17" s="30" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AB17" s="29">
         <v>2.93</v>
@@ -9911,13 +9911,13 @@
         <v>12</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AH17" s="13">
         <v>-0.42</v>
       </c>
       <c r="AI17" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AJ17" s="13">
         <v>-1.7</v>
@@ -9993,7 +9993,7 @@
         <v>77.55</v>
       </c>
       <c r="AI19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -10038,7 +10038,7 @@
         <v>0.23</v>
       </c>
       <c r="AI20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -10524,7 +10524,7 @@
         <v>0.04</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D28" s="7">
         <v>0.33</v>
@@ -10548,7 +10548,7 @@
         <v>-0.04</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L28" s="26">
         <v>-1.31</v>
@@ -10620,7 +10620,7 @@
         <v>0.06</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AJ28" s="7">
         <v>1.1499999999999999</v>
@@ -10640,13 +10640,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B29" s="13">
         <v>-0.26</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D29" s="13">
         <v>-1.35</v>
@@ -10664,13 +10664,13 @@
         <v>94</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J29" s="13">
         <v>-0.01</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="L29" s="13">
         <v>-0.1</v>
@@ -10688,7 +10688,7 @@
         <v>3</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="R29" s="15" t="s">
         <v>29</v>
@@ -10712,13 +10712,13 @@
         <v>29</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Z29" s="15">
         <v>0.08</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AB29" s="15">
         <v>0.75</v>
@@ -10736,13 +10736,13 @@
         <v>12</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AH29" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AJ29" s="15">
         <v>-0.48</v>
@@ -10798,18 +10798,18 @@
   <sheetData>
     <row r="1" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -10926,10 +10926,10 @@
         <v>3.15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>8</v>
@@ -10938,10 +10938,10 @@
         <v>1.56</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>8</v>
@@ -10950,10 +10950,10 @@
         <v>3.71</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>8</v>
@@ -10962,10 +10962,10 @@
         <v>1.4</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>8</v>
@@ -10977,7 +10977,7 @@
         <v>27</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -11368,13 +11368,13 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B16">
         <v>-0.24</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D16">
         <v>-1.36</v>
@@ -11383,13 +11383,13 @@
         <v>0.18</v>
       </c>
       <c r="F16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G16">
         <v>-0.23</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I16">
         <v>-0.81</v>
@@ -11398,13 +11398,13 @@
         <v>0.42</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L16" s="4">
         <v>0.37</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N16" s="4">
         <v>1.99</v>
@@ -11413,13 +11413,13 @@
         <v>0.05</v>
       </c>
       <c r="P16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q16">
         <v>-0.04</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="S16">
         <v>-0.19</v>
@@ -11428,13 +11428,13 @@
         <v>0.85</v>
       </c>
       <c r="U16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="V16">
         <v>0.66</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="X16">
         <v>1.2</v>
@@ -11445,13 +11445,13 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B17">
         <v>-0.23</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D17">
         <v>-1.24</v>
@@ -11460,13 +11460,13 @@
         <v>0.22</v>
       </c>
       <c r="F17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G17">
         <v>-0.11</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I17">
         <v>-0.43</v>
@@ -11475,13 +11475,13 @@
         <v>0.67</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L17" s="4">
         <v>0.76</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N17" s="4">
         <v>3.05</v>
@@ -11490,13 +11490,13 @@
         <v>2E-3</v>
       </c>
       <c r="P17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Q17" s="5">
         <v>0.24</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="S17" s="5">
         <v>1.1599999999999999</v>
@@ -11505,13 +11505,13 @@
         <v>0.25</v>
       </c>
       <c r="U17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="V17">
         <v>0.8</v>
       </c>
       <c r="W17" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="X17">
         <v>1.21</v>
@@ -11522,13 +11522,13 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B18">
         <v>-0.3</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D18">
         <v>-1.82</v>
@@ -11537,13 +11537,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G18">
         <v>-0.22</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I18">
         <v>-0.82</v>
@@ -11552,13 +11552,13 @@
         <v>0.41</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L18" s="4">
         <v>0.62</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N18" s="4">
         <v>3.35</v>
@@ -11567,13 +11567,13 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="P18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Q18" s="5">
         <v>0.28000000000000003</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S18" s="5">
         <v>1.43</v>
@@ -11582,13 +11582,13 @@
         <v>0.15</v>
       </c>
       <c r="U18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="V18">
         <v>0.78</v>
       </c>
       <c r="W18" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X18">
         <v>1.6</v>
@@ -11599,13 +11599,13 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B19">
         <v>-0.03</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D19">
         <v>-0.16</v>
@@ -11614,13 +11614,13 @@
         <v>0.88</v>
       </c>
       <c r="F19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G19">
         <v>-0.11</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I19">
         <v>-0.4</v>
@@ -11629,13 +11629,13 @@
         <v>0.69</v>
       </c>
       <c r="K19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L19">
         <v>0.37</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N19">
         <v>1.74</v>
@@ -11644,13 +11644,13 @@
         <v>0.08</v>
       </c>
       <c r="P19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Q19" s="5">
         <v>0.18</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="S19" s="5">
         <v>0.9</v>
@@ -11659,13 +11659,13 @@
         <v>0.37</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="V19" s="5">
         <v>0.87</v>
       </c>
       <c r="W19" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="X19" s="5">
         <v>1.86</v>
@@ -11676,13 +11676,13 @@
     </row>
     <row r="20" spans="1:25" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B20" s="22">
         <v>-0.79</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D20" s="22">
         <v>-3.04</v>
@@ -11691,13 +11691,13 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G20" s="20">
         <v>-0.47</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I20" s="20">
         <v>-1.64</v>
@@ -11706,13 +11706,13 @@
         <v>0.1</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="L20" s="22">
         <v>0.62</v>
       </c>
       <c r="M20" s="23" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N20" s="22">
         <v>2.04</v>
@@ -11721,13 +11721,13 @@
         <v>0.04</v>
       </c>
       <c r="P20" s="24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q20" s="20">
         <v>0.23</v>
       </c>
       <c r="R20" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="S20" s="20">
         <v>1.07</v>
@@ -11736,13 +11736,13 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="V20" s="24">
         <v>0.6</v>
       </c>
       <c r="W20" s="25" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="X20" s="24">
         <v>1.1399999999999999</v>
@@ -11753,13 +11753,13 @@
     </row>
     <row r="21" spans="1:25" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B21" s="15">
         <v>0.02</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D21" s="15">
         <v>1.1100000000000001</v>
@@ -11768,13 +11768,13 @@
         <v>0.27</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G21" s="15">
         <v>0.02</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I21" s="15">
         <v>0.55000000000000004</v>
@@ -11783,13 +11783,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="K21" s="29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L21" s="29">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N21" s="29">
         <v>-2.9</v>
@@ -11798,13 +11798,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="P21" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q21" s="15">
         <v>-0.03</v>
       </c>
       <c r="R21" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="S21" s="15">
         <v>-1.1200000000000001</v>
@@ -11813,13 +11813,13 @@
         <v>0.26</v>
       </c>
       <c r="U21" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V21" s="15">
         <v>-0.23</v>
       </c>
       <c r="W21" s="16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="X21" s="15">
         <v>-1.4</v>
@@ -11900,10 +11900,10 @@
         <v>1.03</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>8</v>
@@ -11912,10 +11912,10 @@
         <v>0.95</v>
       </c>
       <c r="H24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>8</v>
@@ -11924,10 +11924,10 @@
         <v>0.72</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>8</v>
@@ -11936,10 +11936,10 @@
         <v>0.23</v>
       </c>
       <c r="R24" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="S24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="U24" s="5" t="s">
         <v>8</v>
@@ -11948,10 +11948,10 @@
         <v>1.41</v>
       </c>
       <c r="W24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="X24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -12336,13 +12336,13 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B32" s="7">
         <v>-0.03</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D32" s="7">
         <v>-0.13</v>
@@ -12351,13 +12351,13 @@
         <v>0.89</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G32" s="7">
         <v>-0.01</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I32" s="7">
         <v>-0.05</v>
@@ -12366,13 +12366,13 @@
         <v>0.96</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L32" s="26">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="M32" s="27" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="N32" s="26">
         <v>-0.94</v>
@@ -12381,13 +12381,13 @@
         <v>0.35</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q32" s="7">
         <v>0.14000000000000001</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="S32" s="7">
         <v>0.79</v>
@@ -12396,13 +12396,13 @@
         <v>0.43</v>
       </c>
       <c r="U32" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="V32" s="7">
         <v>0.67</v>
       </c>
       <c r="W32" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="X32" s="7">
         <v>1.1100000000000001</v>
@@ -12413,13 +12413,13 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B33" s="24">
         <v>-0.13</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D33" s="24">
         <v>-0.61</v>
@@ -12428,13 +12428,13 @@
         <v>0.54</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G33" s="20">
         <v>-0.11</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I33" s="20">
         <v>-1.05</v>
@@ -12443,13 +12443,13 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K33" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L33" s="24">
         <v>0.01</v>
       </c>
       <c r="M33" s="25" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="N33" s="24">
         <v>0.08</v>
@@ -12458,13 +12458,13 @@
         <v>0.93</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Q33" s="24">
         <v>0.14000000000000001</v>
       </c>
       <c r="R33" s="25" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="S33" s="24">
         <v>0.79</v>
@@ -12473,13 +12473,13 @@
         <v>0.43</v>
       </c>
       <c r="U33" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="V33" s="20">
         <v>1.3</v>
       </c>
       <c r="W33" s="21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="X33" s="20">
         <v>1.78</v>
@@ -12490,13 +12490,13 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B34" s="24">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D34" s="24">
         <v>-0.44</v>
@@ -12505,13 +12505,13 @@
         <v>0.66</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G34" s="24">
         <v>0</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I34" s="24">
         <v>0.02</v>
@@ -12520,13 +12520,13 @@
         <v>0.99</v>
       </c>
       <c r="K34" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L34" s="24">
         <v>-0.03</v>
       </c>
       <c r="M34" s="25" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="N34" s="24">
         <v>-0.43</v>
@@ -12535,13 +12535,13 @@
         <v>0.67</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Q34" s="24">
         <v>0.09</v>
       </c>
       <c r="R34" s="25" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="S34" s="24">
         <v>0.56000000000000005</v>
@@ -12550,13 +12550,13 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="U34" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="V34" s="24">
         <v>0.8</v>
       </c>
       <c r="W34" s="25" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="X34" s="24">
         <v>1.51</v>
@@ -12567,13 +12567,13 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B35" s="20">
         <v>-0.32</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D35" s="20">
         <v>-1.82</v>
@@ -12582,13 +12582,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G35" s="24">
         <v>-0.01</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I35" s="24">
         <v>-0.13</v>
@@ -12597,13 +12597,13 @@
         <v>0.89</v>
       </c>
       <c r="K35" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L35" s="24">
         <v>0.04</v>
       </c>
       <c r="M35" s="25" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="N35" s="24">
         <v>0.45</v>
@@ -12612,13 +12612,13 @@
         <v>0.66</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Q35" s="24">
         <v>0.08</v>
       </c>
       <c r="R35" s="25" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="S35" s="24">
         <v>0.47</v>
@@ -12627,13 +12627,13 @@
         <v>0.64</v>
       </c>
       <c r="U35" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="V35" s="24">
         <v>0.56999999999999995</v>
       </c>
       <c r="W35" s="25" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="X35" s="24">
         <v>1.1100000000000001</v>
@@ -12644,13 +12644,13 @@
     </row>
     <row r="36" spans="1:25" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B36" s="24">
         <v>0.08</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D36" s="24">
         <v>0.27</v>
@@ -12659,13 +12659,13 @@
         <v>0.79</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G36" s="20">
         <v>0.09</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I36" s="20">
         <v>0.72</v>
@@ -12674,13 +12674,13 @@
         <v>0.47</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="L36" s="24">
         <v>0.22</v>
       </c>
       <c r="M36" s="25" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="N36" s="24">
         <v>1.32</v>
@@ -12689,13 +12689,13 @@
         <v>0.19</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q36" s="24">
         <v>0.1</v>
       </c>
       <c r="R36" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="S36" s="24">
         <v>0.54</v>
@@ -12704,13 +12704,13 @@
         <v>0.59</v>
       </c>
       <c r="U36" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="V36" s="24">
         <v>0.47</v>
       </c>
       <c r="W36" s="25" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="X36" s="24">
         <v>0.86</v>
@@ -12721,13 +12721,13 @@
     </row>
     <row r="37" spans="1:25" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B37" s="15">
         <v>0.02</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D37" s="15">
         <v>0.53</v>
@@ -12736,13 +12736,13 @@
         <v>0.6</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G37" s="15">
         <v>-0.01</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I37" s="15">
         <v>-0.28000000000000003</v>
@@ -12751,13 +12751,13 @@
         <v>0.78</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L37" s="15">
         <v>0</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="N37" s="15">
         <v>0.16</v>
@@ -12766,13 +12766,13 @@
         <v>0.87</v>
       </c>
       <c r="P37" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q37" s="15">
         <v>-0.01</v>
       </c>
       <c r="R37" s="16" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="S37" s="15">
         <v>-0.4</v>
@@ -12781,13 +12781,13 @@
         <v>0.69</v>
       </c>
       <c r="U37" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V37" s="15">
         <v>-0.25</v>
       </c>
       <c r="W37" s="16" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="X37" s="15">
         <v>-1.36</v>

</xml_diff>